<commit_message>
fix p3 and p4
</commit_message>
<xml_diff>
--- a/test_fun/p3_phase2_SEGA23.xlsx
+++ b/test_fun/p3_phase2_SEGA23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gian/Documents/SEGA2023/test_fun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C1E46-3EFB-B045-874F-B5561E830894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED4B3CF-3374-3A43-8794-7FF4C1A2C02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45760" yWindow="2200" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2026,7 +2026,7 @@
         <v>2.001757</v>
       </c>
       <c r="D2" s="3">
-        <v>9.02</v>
+        <v>172.52</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -2042,7 +2042,7 @@
         <v>2.781425</v>
       </c>
       <c r="D3" s="3">
-        <v>10.23</v>
+        <v>97.7</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -2058,7 +2058,7 @@
         <v>8.9938830000000003</v>
       </c>
       <c r="D4" s="3">
-        <v>10.130000000000001</v>
+        <v>141.12</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2074,7 +2074,7 @@
         <v>5.5390050000000004</v>
       </c>
       <c r="D5" s="3">
-        <v>10.62</v>
+        <v>132.13999999999999</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2090,7 +2090,7 @@
         <v>11.001054999999999</v>
       </c>
       <c r="D6" s="3">
-        <v>9.02</v>
+        <v>101.5</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>

</xml_diff>